<commit_message>
correct the yaml and json file of miaca
</commit_message>
<xml_diff>
--- a/templates/miaca/MIACA_template.xlsx
+++ b/templates/miaca/MIACA_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/apple/ToxRSCat/templates/miaca/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEB87343-B4E6-C14E-90BA-2F344727BAA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BF3B41A-C021-5F4B-AA5B-6759A190475B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15720" activeTab="1" xr2:uid="{4C05F035-5B59-104F-A647-E8EAB47C9886}"/>
   </bookViews>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="248">
   <si>
     <t>description</t>
   </si>
@@ -392,9 +392,6 @@
     <t>sample_identifier</t>
   </si>
   <si>
-    <t xml:space="preserve"> cellDensity</t>
-  </si>
-  <si>
     <t xml:space="preserve"> transgene/genetic manipulations, e.g. stably transfected, induced</t>
   </si>
   <si>
@@ -795,6 +792,24 @@
   </si>
   <si>
     <t>Sample.subject_identifier</t>
+  </si>
+  <si>
+    <t>TBD.stem_cell</t>
+  </si>
+  <si>
+    <t>TBD.cell_line</t>
+  </si>
+  <si>
+    <t>date.culture_vessel</t>
+  </si>
+  <si>
+    <t>date.medium</t>
+  </si>
+  <si>
+    <t>date.treatment</t>
+  </si>
+  <si>
+    <t>date.sample_details</t>
   </si>
 </sst>
 </file>
@@ -826,7 +841,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -836,6 +851,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -882,7 +903,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
@@ -914,6 +935,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1307,8 +1332,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C25A47E7-C24D-194E-BA2A-C4B34C2EC6AD}">
   <dimension ref="A1:T92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D58" zoomScale="112" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="O21" sqref="O21"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="93" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="D92" sqref="D92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1393,7 +1418,7 @@
         <v>88</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D2" s="11" t="s">
         <v>87</v>
@@ -1418,7 +1443,7 @@
       <c r="P2" s="11"/>
       <c r="Q2" s="11"/>
       <c r="R2" s="11" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="S2" s="11"/>
       <c r="T2" s="11"/>
@@ -1443,7 +1468,7 @@
         <v>39</v>
       </c>
       <c r="R3" s="4" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="4" spans="1:20" ht="51" x14ac:dyDescent="0.2">
@@ -1495,13 +1520,13 @@
         <v>1</v>
       </c>
       <c r="L5" s="4" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="N5" s="4" t="b">
         <v>1</v>
       </c>
       <c r="R5" s="4" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="6" spans="1:20" ht="68" x14ac:dyDescent="0.2">
@@ -1521,7 +1546,7 @@
         <v>103</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I6" s="4" t="b">
         <v>1</v>
@@ -1553,7 +1578,7 @@
         <v>103</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="I7" s="4" t="b">
         <v>1</v>
@@ -1588,7 +1613,7 @@
         <v>103</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I8" s="4" t="b">
         <v>1</v>
@@ -1600,7 +1625,7 @@
         <v>42</v>
       </c>
       <c r="R8" s="4" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="9" spans="1:20" ht="119" x14ac:dyDescent="0.2">
@@ -1626,7 +1651,7 @@
         <v>1</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="L9" s="4" t="s">
         <v>43</v>
@@ -1658,7 +1683,7 @@
         <v>1</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="L10" s="4" t="s">
         <v>44</v>
@@ -1684,7 +1709,7 @@
         <v>103</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I11" s="4" t="b">
         <v>1</v>
@@ -1751,7 +1776,7 @@
         <v>1</v>
       </c>
       <c r="K13" s="4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="L13" s="4" t="s">
         <v>47</v>
@@ -1771,7 +1796,7 @@
         <v>37</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E14" s="4" t="s">
         <v>106</v>
@@ -1783,13 +1808,13 @@
         <v>1</v>
       </c>
       <c r="K14" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="N14" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="R14" s="4" t="s">
         <v>213</v>
-      </c>
-      <c r="N14" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="R14" s="4" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="15" spans="1:20" ht="17" x14ac:dyDescent="0.2">
@@ -1838,7 +1863,7 @@
         <v>103</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="I16" s="4" t="b">
         <v>1</v>
@@ -1889,7 +1914,7 @@
       <c r="F18" s="6"/>
       <c r="G18" s="6"/>
       <c r="H18" s="6" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="I18" s="6" t="b">
         <v>1</v>
@@ -1916,7 +1941,7 @@
         <v>88</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D19" s="11" t="s">
         <v>89</v>
@@ -1941,33 +1966,46 @@
       <c r="P19" s="11"/>
       <c r="Q19" s="11"/>
       <c r="R19" s="11" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="S19" s="11"/>
       <c r="T19" s="11"/>
     </row>
-    <row r="20" spans="1:20" ht="17" x14ac:dyDescent="0.2">
-      <c r="A20" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="B20" s="4" t="s">
+    <row r="20" spans="1:20" s="16" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A20" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="B20" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="C20" s="4" t="s">
-        <v>238</v>
-      </c>
-      <c r="D20" s="4" t="s">
+      <c r="C20" s="15" t="s">
+        <v>237</v>
+      </c>
+      <c r="D20" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="E20" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="O20" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="R20" s="4" t="s">
-        <v>210</v>
-      </c>
+      <c r="E20" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="F20" s="15"/>
+      <c r="G20" s="15"/>
+      <c r="H20" s="15"/>
+      <c r="I20" s="15"/>
+      <c r="J20" s="15"/>
+      <c r="K20" s="15"/>
+      <c r="L20" s="15"/>
+      <c r="M20" s="15"/>
+      <c r="N20" s="15"/>
+      <c r="O20" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="P20" s="15"/>
+      <c r="Q20" s="15"/>
+      <c r="R20" s="15" t="s">
+        <v>209</v>
+      </c>
+      <c r="S20" s="15"/>
+      <c r="T20" s="15"/>
     </row>
     <row r="21" spans="1:20" ht="68" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
@@ -1977,16 +2015,16 @@
         <v>86</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E21" s="4" t="s">
         <v>103</v>
       </c>
       <c r="L21" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="P21" s="4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="Q21" s="5" t="s">
         <v>70</v>
@@ -2009,19 +2047,19 @@
         <v>106</v>
       </c>
       <c r="K22" s="4" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="L22" s="4" t="s">
         <v>73</v>
       </c>
       <c r="P22" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="Q22" s="5" t="s">
         <v>70</v>
       </c>
       <c r="R22" s="4" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="23" spans="1:20" ht="323" x14ac:dyDescent="0.2">
@@ -2041,13 +2079,13 @@
         <v>106</v>
       </c>
       <c r="K23" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="L23" s="4" t="s">
         <v>74</v>
       </c>
       <c r="R23" s="4" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="24" spans="1:20" ht="17" x14ac:dyDescent="0.2">
@@ -2067,10 +2105,10 @@
         <v>106</v>
       </c>
       <c r="K24" s="4" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="R24" s="4" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="25" spans="1:20" ht="34" x14ac:dyDescent="0.2">
@@ -2078,28 +2116,28 @@
         <v>84</v>
       </c>
       <c r="B25" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="C25" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="C25" s="4" t="s">
-        <v>122</v>
-      </c>
       <c r="D25" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E25" s="4" t="s">
         <v>106</v>
       </c>
       <c r="K25" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="P25" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="Q25" s="5" t="s">
         <v>70</v>
       </c>
       <c r="R25" s="4" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="26" spans="1:20" ht="85" x14ac:dyDescent="0.2">
@@ -2107,23 +2145,23 @@
         <v>84</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E26" s="4" t="s">
         <v>103</v>
       </c>
       <c r="K26" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="Q26" s="3"/>
       <c r="R26" s="4" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="27" spans="1:20" ht="17" x14ac:dyDescent="0.2">
@@ -2131,13 +2169,13 @@
         <v>84</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E27" s="4" t="s">
         <v>103</v>
@@ -2149,7 +2187,7 @@
         <v>84</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>94</v>
@@ -2161,11 +2199,11 @@
         <v>106</v>
       </c>
       <c r="K28" s="4" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="Q28" s="3"/>
       <c r="R28" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="29" spans="1:20" ht="17" x14ac:dyDescent="0.2">
@@ -2173,7 +2211,7 @@
         <v>84</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>93</v>
@@ -2185,11 +2223,11 @@
         <v>106</v>
       </c>
       <c r="K29" s="4" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="Q29" s="3"/>
       <c r="R29" s="4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="30" spans="1:20" ht="17" x14ac:dyDescent="0.2">
@@ -2197,13 +2235,13 @@
         <v>84</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E30" s="4" t="s">
         <v>104</v>
@@ -2224,13 +2262,13 @@
         <v>84</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E31" s="4" t="s">
         <v>104</v>
@@ -2248,41 +2286,41 @@
         <v>84</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E32" s="4" t="s">
         <v>103</v>
       </c>
       <c r="Q32" s="3"/>
     </row>
-    <row r="33" spans="1:18" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:18" ht="409.5" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
         <v>84</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E33" s="4" t="s">
         <v>106</v>
       </c>
       <c r="K33" s="4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="Q33" s="3"/>
       <c r="R33" s="4" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="34" spans="1:18" ht="17" x14ac:dyDescent="0.2">
@@ -2290,13 +2328,13 @@
         <v>84</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E34" s="4" t="s">
         <v>103</v>
@@ -2308,26 +2346,26 @@
         <v>84</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E35" s="4" t="s">
         <v>103</v>
       </c>
       <c r="K35" s="4" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="L35" s="4" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="Q35" s="3"/>
       <c r="R35" s="4" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="36" spans="1:18" ht="17" x14ac:dyDescent="0.2">
@@ -2335,23 +2373,23 @@
         <v>84</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E36" s="4" t="s">
         <v>103</v>
       </c>
       <c r="K36" s="4" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="Q36" s="3"/>
       <c r="R36" s="4" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="37" spans="1:18" ht="17" x14ac:dyDescent="0.2">
@@ -2359,20 +2397,20 @@
         <v>84</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E37" s="4" t="s">
         <v>103</v>
       </c>
       <c r="Q37" s="3"/>
       <c r="R37" s="4" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="38" spans="1:18" ht="68" x14ac:dyDescent="0.2">
@@ -2380,22 +2418,22 @@
         <v>84</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E38" s="4" t="s">
         <v>103</v>
       </c>
       <c r="L38" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="P38" s="4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="39" spans="1:18" ht="51" x14ac:dyDescent="0.2">
@@ -2403,13 +2441,13 @@
         <v>84</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E39" s="4" t="s">
         <v>106</v>
@@ -2421,13 +2459,13 @@
         <v>1</v>
       </c>
       <c r="K39" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="L39" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="P39" s="4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="40" spans="1:18" ht="51" x14ac:dyDescent="0.2">
@@ -2435,13 +2473,13 @@
         <v>84</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E40" s="4" t="s">
         <v>106</v>
@@ -2453,13 +2491,13 @@
         <v>1</v>
       </c>
       <c r="K40" s="4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="L40" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="P40" s="4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="Q40" s="5"/>
     </row>
@@ -2468,13 +2506,13 @@
         <v>84</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E41" s="4" t="s">
         <v>103</v>
@@ -2486,13 +2524,13 @@
         <v>84</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E42" s="4" t="s">
         <v>103</v>
@@ -2504,10 +2542,13 @@
         <v>84</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>156</v>
+        <v>242</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>155</v>
       </c>
       <c r="E43" s="4" t="s">
         <v>103</v>
@@ -2519,10 +2560,13 @@
         <v>84</v>
       </c>
       <c r="B44" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>243</v>
+      </c>
+      <c r="D44" s="4" t="s">
         <v>155</v>
-      </c>
-      <c r="C44" s="4" t="s">
-        <v>156</v>
       </c>
       <c r="E44" s="4" t="s">
         <v>103</v>
@@ -2534,10 +2578,10 @@
         <v>84</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>91</v>
+        <v>244</v>
       </c>
       <c r="D45" s="4" t="s">
         <v>91</v>
@@ -2552,25 +2596,25 @@
         <v>84</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E46" s="4" t="s">
         <v>106</v>
       </c>
       <c r="K46" s="4" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="L46" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="P46" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="47" spans="1:18" ht="17" x14ac:dyDescent="0.2">
@@ -2578,19 +2622,19 @@
         <v>84</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E47" s="4" t="s">
         <v>103</v>
       </c>
       <c r="P47" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="48" spans="1:18" ht="34" x14ac:dyDescent="0.2">
@@ -2598,13 +2642,13 @@
         <v>84</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E48" s="4" t="s">
         <v>104</v>
@@ -2616,10 +2660,10 @@
         <v>384</v>
       </c>
       <c r="L48" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="P48" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="49" spans="1:18" ht="34" x14ac:dyDescent="0.2">
@@ -2627,13 +2671,13 @@
         <v>84</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E49" s="4" t="s">
         <v>105</v>
@@ -2642,10 +2686,10 @@
         <v>0</v>
       </c>
       <c r="L49" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="P49" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="50" spans="1:18" ht="17" x14ac:dyDescent="0.2">
@@ -2653,13 +2697,13 @@
         <v>84</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E50" s="4" t="s">
         <v>105</v>
@@ -2668,10 +2712,10 @@
         <v>0</v>
       </c>
       <c r="L50" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="P50" s="4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="51" spans="1:18" ht="17" x14ac:dyDescent="0.2">
@@ -2679,19 +2723,19 @@
         <v>84</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E51" s="4" t="s">
         <v>103</v>
       </c>
       <c r="R51" s="4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="52" spans="1:18" ht="17" x14ac:dyDescent="0.2">
@@ -2699,19 +2743,19 @@
         <v>84</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E52" s="4" t="s">
         <v>103</v>
       </c>
       <c r="R52" s="4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="53" spans="1:18" ht="17" x14ac:dyDescent="0.2">
@@ -2719,10 +2763,10 @@
         <v>84</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E53" s="4" t="s">
         <v>105</v>
@@ -2736,10 +2780,10 @@
         <v>84</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E54" s="4" t="s">
         <v>91</v>
@@ -2750,16 +2794,16 @@
         <v>84</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>108</v>
+        <v>143</v>
       </c>
       <c r="E55" s="4" t="s">
         <v>103</v>
       </c>
       <c r="P55" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="56" spans="1:18" ht="17" x14ac:dyDescent="0.2">
@@ -2767,13 +2811,13 @@
         <v>84</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E56" s="4" t="s">
         <v>103</v>
@@ -2784,13 +2828,13 @@
         <v>84</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E57" s="4" t="s">
         <v>103</v>
@@ -2801,13 +2845,13 @@
         <v>84</v>
       </c>
       <c r="B58" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="C58" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="C58" s="4" t="s">
-        <v>137</v>
-      </c>
       <c r="D58" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E58" s="4" t="s">
         <v>105</v>
@@ -2827,13 +2871,13 @@
         <v>84</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E59" s="4" t="s">
         <v>105</v>
@@ -2850,13 +2894,13 @@
         <v>84</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E60" s="4" t="s">
         <v>103</v>
@@ -2873,13 +2917,13 @@
         <v>84</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D61" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E61" s="4" t="s">
         <v>103</v>
@@ -2896,10 +2940,10 @@
         <v>84</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>91</v>
+        <v>245</v>
       </c>
       <c r="D62" s="4" t="s">
         <v>91</v>
@@ -2913,13 +2957,13 @@
         <v>84</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D63" s="4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E63" s="4" t="s">
         <v>103</v>
@@ -2930,128 +2974,142 @@
         <v>84</v>
       </c>
       <c r="B64" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="C64" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="C64" s="4" t="s">
+      <c r="D64" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="E64" s="4" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="65" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+      <c r="A65" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B65" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="C65" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="D64" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="E64" s="4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="65" spans="1:17" ht="17" x14ac:dyDescent="0.2">
-      <c r="A65" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="B65" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="C65" s="4" t="s">
+      <c r="E65" s="4" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="66" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+      <c r="A66" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B66" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="C66" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="E65" s="4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="66" spans="1:17" ht="17" x14ac:dyDescent="0.2">
-      <c r="A66" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="B66" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="C66" s="4" t="s">
+      <c r="E66" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q66" s="3"/>
+    </row>
+    <row r="67" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+      <c r="A67" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B67" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="C67" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="E66" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="Q66" s="3"/>
-    </row>
-    <row r="67" spans="1:17" ht="17" x14ac:dyDescent="0.2">
-      <c r="A67" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="B67" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="C67" s="4" t="s">
+      <c r="E67" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q67" s="3"/>
+    </row>
+    <row r="68" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+      <c r="A68" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B68" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="C68" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="E67" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="Q67" s="3"/>
-    </row>
-    <row r="68" spans="1:17" ht="17" x14ac:dyDescent="0.2">
-      <c r="A68" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="B68" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="C68" s="4" t="s">
+      <c r="E68" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q68" s="3"/>
+    </row>
+    <row r="69" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+      <c r="A69" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B69" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="C69" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="E68" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="Q68" s="3"/>
-    </row>
-    <row r="69" spans="1:17" ht="17" x14ac:dyDescent="0.2">
-      <c r="A69" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="B69" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="C69" s="4" t="s">
+      <c r="E69" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q69" s="3"/>
+    </row>
+    <row r="70" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+      <c r="A70" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B70" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="C70" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="E69" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="Q69" s="3"/>
-    </row>
-    <row r="70" spans="1:17" ht="17" x14ac:dyDescent="0.2">
-      <c r="A70" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="B70" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="C70" s="4" t="s">
-        <v>152</v>
-      </c>
       <c r="E70" s="4" t="s">
         <v>103</v>
       </c>
       <c r="Q70" s="3"/>
     </row>
-    <row r="71" spans="1:17" ht="17" x14ac:dyDescent="0.2">
-      <c r="A71" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="B71" s="4" t="s">
+    <row r="71" spans="1:20" s="16" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A71" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="B71" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="C71" s="4" t="s">
-        <v>237</v>
-      </c>
-      <c r="D71" s="4" t="s">
+      <c r="C71" s="15" t="s">
+        <v>236</v>
+      </c>
+      <c r="D71" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="E71" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="N71" s="4" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="72" spans="1:17" ht="68" x14ac:dyDescent="0.2">
+      <c r="E71" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="F71" s="15"/>
+      <c r="G71" s="15"/>
+      <c r="H71" s="15"/>
+      <c r="I71" s="15"/>
+      <c r="J71" s="15"/>
+      <c r="K71" s="15"/>
+      <c r="L71" s="15"/>
+      <c r="M71" s="15"/>
+      <c r="N71" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="O71" s="15"/>
+      <c r="P71" s="15"/>
+      <c r="Q71" s="15"/>
+      <c r="R71" s="15"/>
+      <c r="S71" s="15"/>
+      <c r="T71" s="15"/>
+    </row>
+    <row r="72" spans="1:20" ht="68" x14ac:dyDescent="0.2">
       <c r="A72" s="4" t="s">
         <v>84</v>
       </c>
@@ -3059,19 +3117,19 @@
         <v>95</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D72" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E72" s="4" t="s">
         <v>103</v>
       </c>
       <c r="L72" s="4" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="73" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="73" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A73" s="4" t="s">
         <v>84</v>
       </c>
@@ -3079,16 +3137,16 @@
         <v>95</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D73" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E73" s="4" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="74" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A74" s="4" t="s">
         <v>84</v>
       </c>
@@ -3096,13 +3154,16 @@
         <v>95</v>
       </c>
       <c r="C74" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="D74" s="4" t="s">
         <v>91</v>
       </c>
       <c r="E74" s="4" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="75" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A75" s="4" t="s">
         <v>84</v>
       </c>
@@ -3110,13 +3171,13 @@
         <v>95</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E75" s="4" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="76" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A76" s="4" t="s">
         <v>84</v>
       </c>
@@ -3124,13 +3185,13 @@
         <v>95</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E76" s="4" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="77" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A77" s="4" t="s">
         <v>84</v>
       </c>
@@ -3138,13 +3199,13 @@
         <v>95</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E77" s="4" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="78" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A78" s="4" t="s">
         <v>84</v>
       </c>
@@ -3152,13 +3213,13 @@
         <v>95</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E78" s="4" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="79" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A79" s="4" t="s">
         <v>84</v>
       </c>
@@ -3172,7 +3233,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="80" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A80" s="4" t="s">
         <v>84</v>
       </c>
@@ -3236,7 +3297,7 @@
         <v>88</v>
       </c>
       <c r="C84" s="13" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D84" s="13" t="s">
         <v>107</v>
@@ -3264,45 +3325,73 @@
       <c r="S84" s="13"/>
       <c r="T84" s="13"/>
     </row>
-    <row r="85" spans="1:20" ht="17" x14ac:dyDescent="0.2">
-      <c r="A85" s="4" t="s">
+    <row r="85" spans="1:20" s="16" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A85" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="B85" s="4" t="s">
+      <c r="B85" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="C85" s="4" t="s">
+      <c r="C85" s="15" t="s">
+        <v>240</v>
+      </c>
+      <c r="D85" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="E85" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="F85" s="15"/>
+      <c r="G85" s="15"/>
+      <c r="H85" s="15"/>
+      <c r="I85" s="15"/>
+      <c r="J85" s="15"/>
+      <c r="K85" s="15"/>
+      <c r="L85" s="15"/>
+      <c r="M85" s="15"/>
+      <c r="N85" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="O85" s="15"/>
+      <c r="P85" s="15"/>
+      <c r="Q85" s="15"/>
+      <c r="R85" s="15"/>
+      <c r="S85" s="15"/>
+      <c r="T85" s="15"/>
+    </row>
+    <row r="86" spans="1:20" s="16" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A86" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="B86" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="C86" s="15" t="s">
         <v>241</v>
       </c>
-      <c r="D85" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="E85" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="N85" s="4" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="86" spans="1:20" ht="17" x14ac:dyDescent="0.2">
-      <c r="A86" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="B86" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="C86" s="4" t="s">
-        <v>242</v>
-      </c>
-      <c r="D86" s="4" t="s">
+      <c r="D86" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="E86" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="O86" s="4" t="b">
-        <v>1</v>
-      </c>
+      <c r="E86" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="F86" s="15"/>
+      <c r="G86" s="15"/>
+      <c r="H86" s="15"/>
+      <c r="I86" s="15"/>
+      <c r="J86" s="15"/>
+      <c r="K86" s="15"/>
+      <c r="L86" s="15"/>
+      <c r="M86" s="15"/>
+      <c r="N86" s="15"/>
+      <c r="O86" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="P86" s="15"/>
+      <c r="Q86" s="15"/>
+      <c r="R86" s="15"/>
+      <c r="S86" s="15"/>
+      <c r="T86" s="15"/>
     </row>
     <row r="87" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A87" s="4" t="s">
@@ -3312,6 +3401,9 @@
         <v>102</v>
       </c>
       <c r="C87" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="D87" s="4" t="s">
         <v>91</v>
       </c>
       <c r="E87" s="4" t="s">
@@ -3326,16 +3418,16 @@
         <v>102</v>
       </c>
       <c r="C88" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D88" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E88" s="4" t="s">
         <v>103</v>
       </c>
       <c r="L88" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="89" spans="1:20" ht="17" x14ac:dyDescent="0.2">
@@ -3360,13 +3452,13 @@
         <v>30</v>
       </c>
       <c r="B90" s="4" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C90" s="4" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E90" s="4" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="91" spans="1:20" ht="34" x14ac:dyDescent="0.2">
@@ -3374,13 +3466,13 @@
         <v>84</v>
       </c>
       <c r="B91" s="4" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C91" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E91" s="4" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="92" spans="1:20" ht="34" x14ac:dyDescent="0.2">
@@ -3388,13 +3480,13 @@
         <v>85</v>
       </c>
       <c r="B92" s="4" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C92" s="4" t="s">
+        <v>233</v>
+      </c>
+      <c r="E92" s="4" t="s">
         <v>234</v>
-      </c>
-      <c r="E92" s="4" t="s">
-        <v>235</v>
       </c>
     </row>
   </sheetData>

</xml_diff>